<commit_message>
Revert "Revert "convert_SINGLE_RES, convert_SECONDARY_RES""
This reverts commit e12a49309fff2313d1f7071ebdb9d80e8dff0ad4.
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/mapping_BUILDING_USE_RATIO.xlsx
+++ b/remap_ville_plugin/mapping_BUILDING_USE_RATIO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D7E1BA-D48F-43E7-984F-1F6D103AB378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D712D0A-5948-4C6B-9C03-A58463FF6297}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{1C1C4709-675E-44E3-8DFB-69CCE1239E02}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="4" xr2:uid="{1C1C4709-675E-44E3-8DFB-69CCE1239E02}"/>
   </bookViews>
   <sheets>
     <sheet name="URB_2040" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="31">
   <si>
     <t>Scenario</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>PUN</t>
+  </si>
+  <si>
+    <t>3871-Klosters-Serneus</t>
+  </si>
+  <si>
+    <t>SECONDARY_RES</t>
+  </si>
+  <si>
+    <t>place-holder</t>
   </si>
 </sst>
 </file>
@@ -975,7 +984,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2238,14 +2247,293 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF5F5E8-3230-403E-9E7C-AC711AEAABE3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.23108195768918199</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.38686405146896702</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.38205399084184999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3.6646807576113202E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.6342989499780301E-2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.5570572178525401E-2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.33903020185543298</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.6835319398836101E-2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>3.7914274791353798E-3</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.119932655617689</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>1.16452677067942E-2</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.79631712669015731</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.20368287330984264</v>
+      </c>
+      <c r="D3" s="2">
+        <v>7.0260787952819093E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.6001254746840204E-3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6.1438286293753683E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7.3730978652184392E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.7383178134777463E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>5.9766633200037389E-3</v>
+      </c>
+      <c r="L3" s="2">
+        <v>6.1810883670063927E-3</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>2.5160393100302197E-2</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>1.4155679239981914E-2</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.23108195768918199</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.38686405146896702</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.38205399084184999</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.6646807576113202E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2.6342989499780301E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.5570572178525401E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.33903020185543298</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.6835319398836101E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3.7914274791353798E-3</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.119932655617689</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1.16452677067942E-2</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E8" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2254,7 +2542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523C6DC8-E5AC-4E32-B877-8A8AF64848B7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>